<commit_message>
Updated Index to include stylized d3 chart, next step adjusting scale and dropping them all in the same place
</commit_message>
<xml_diff>
--- a/Assignments/FinalProject/Radigan/Project/files/numbers.xlsx
+++ b/Assignments/FinalProject/Radigan/Project/files/numbers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Sets</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Team +/-</t>
+  </si>
+  <si>
+    <t>j</t>
   </si>
 </sst>
 </file>
@@ -398,14 +401,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr>
+                <a:latin typeface="Roboto Condensed Light"/>
+                <a:cs typeface="Roboto Condensed Light"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Roboto Condensed Light"/>
+                <a:cs typeface="Roboto Condensed Light"/>
+              </a:rPr>
               <a:t>Robinson vs.</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Roboto Condensed Light"/>
+                <a:cs typeface="Roboto Condensed Light"/>
+              </a:rPr>
               <a:t> The Team (Hitting %)</a:t>
             </a:r>
           </a:p>
@@ -650,11 +662,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2129533272"/>
-        <c:axId val="-2129523528"/>
+        <c:axId val="2127888088"/>
+        <c:axId val="2129438920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2129533272"/>
+        <c:axId val="2127888088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -663,7 +675,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129523528"/>
+        <c:crossAx val="2129438920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -671,7 +683,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129523528"/>
+        <c:axId val="2129438920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -682,15 +694,43 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129533272"/>
+        <c:crossAx val="2127888088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.58220502901354"/>
+          <c:y val="0.753012590629142"/>
+          <c:w val="0.135396518375242"/>
+          <c:h val="0.0994203632961721"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -725,17 +765,29 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr>
+                <a:latin typeface="Roboto Condensed Light"/>
+                <a:cs typeface="Roboto Condensed Light"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Roboto Condensed Light"/>
+                <a:cs typeface="Roboto Condensed Light"/>
+              </a:rPr>
               <a:t>Robinson's</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Roboto Condensed Light"/>
+                <a:cs typeface="Roboto Condensed Light"/>
+              </a:rPr>
               <a:t> HPR vs. Team's Result (In sets +/-)</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US">
+              <a:latin typeface="Roboto Condensed Light"/>
+              <a:cs typeface="Roboto Condensed Light"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -978,20 +1030,20 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2126669272"/>
-        <c:axId val="-2128838552"/>
+        <c:axId val="2129795992"/>
+        <c:axId val="2129798968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2126669272"/>
+        <c:axId val="2129795992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128838552"/>
+        <c:crossAx val="2129798968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -999,18 +1051,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128838552"/>
+        <c:axId val="2129798968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126669272"/>
+        <c:crossAx val="2129795992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1102,8 +1154,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -3188,14 +3240,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="N33"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="33" spans="14:14">
+      <c r="N33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>

</xml_diff>